<commit_message>
Parallel For Sundaram home added
</commit_message>
<xml_diff>
--- a/CW2/#Results/#Comparison.xlsx
+++ b/CW2/#Results/#Comparison.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40168766\Documents\GitHub\ConcurrentAndParallelSystems\CW2\#Results\Sequentials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Uni\Year-4\ConcurrentAndParallelSystems\ConcurrentAndParallelSystems\CW2\#Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -492,11 +492,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P34" sqref="P34"/>
+      <selection activeCell="R4" sqref="R4:R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,7 +678,9 @@
       </c>
       <c r="L4" s="2"/>
       <c r="O4" s="2"/>
-      <c r="R4" s="2"/>
+      <c r="R4">
+        <v>718272</v>
+      </c>
       <c r="S4" s="2"/>
       <c r="V4" s="2"/>
       <c r="Y4" s="2"/>
@@ -708,7 +710,9 @@
       </c>
       <c r="L5" s="2"/>
       <c r="O5" s="2"/>
-      <c r="R5" s="2"/>
+      <c r="R5">
+        <v>724651</v>
+      </c>
       <c r="S5" s="2"/>
       <c r="V5" s="2"/>
       <c r="Y5" s="2"/>
@@ -738,7 +742,9 @@
       </c>
       <c r="L6" s="2"/>
       <c r="O6" s="2"/>
-      <c r="R6" s="2"/>
+      <c r="R6">
+        <v>729076</v>
+      </c>
       <c r="S6" s="2"/>
       <c r="V6" s="2"/>
       <c r="Y6" s="2"/>
@@ -768,7 +774,9 @@
       </c>
       <c r="L7" s="2"/>
       <c r="O7" s="2"/>
-      <c r="R7" s="2"/>
+      <c r="R7">
+        <v>728885</v>
+      </c>
       <c r="S7" s="2"/>
       <c r="V7" s="2"/>
       <c r="Y7" s="2"/>
@@ -798,7 +806,9 @@
       </c>
       <c r="L8" s="2"/>
       <c r="O8" s="2"/>
-      <c r="R8" s="2"/>
+      <c r="R8">
+        <v>722310</v>
+      </c>
       <c r="S8" s="2"/>
       <c r="V8" s="2"/>
       <c r="Y8" s="2"/>
@@ -828,7 +838,9 @@
       </c>
       <c r="L9" s="2"/>
       <c r="O9" s="2"/>
-      <c r="R9" s="2"/>
+      <c r="R9">
+        <v>722949</v>
+      </c>
       <c r="S9" s="2"/>
       <c r="V9" s="2"/>
       <c r="Y9" s="2"/>
@@ -858,7 +870,9 @@
       </c>
       <c r="L10" s="2"/>
       <c r="O10" s="2"/>
-      <c r="R10" s="2"/>
+      <c r="R10">
+        <v>724420</v>
+      </c>
       <c r="S10" s="2"/>
       <c r="V10" s="2"/>
       <c r="Y10" s="2"/>
@@ -888,7 +902,9 @@
       </c>
       <c r="L11" s="2"/>
       <c r="O11" s="2"/>
-      <c r="R11" s="2"/>
+      <c r="R11">
+        <v>722250</v>
+      </c>
       <c r="S11" s="2"/>
       <c r="V11" s="2"/>
       <c r="Y11" s="2"/>
@@ -918,7 +934,9 @@
       </c>
       <c r="L12" s="2"/>
       <c r="O12" s="2"/>
-      <c r="R12" s="2"/>
+      <c r="R12">
+        <v>814343</v>
+      </c>
       <c r="S12" s="2"/>
       <c r="V12" s="2"/>
       <c r="Y12" s="2"/>
@@ -948,7 +966,9 @@
       </c>
       <c r="L13" s="2"/>
       <c r="O13" s="2"/>
-      <c r="R13" s="2"/>
+      <c r="R13">
+        <v>795331</v>
+      </c>
       <c r="S13" s="2"/>
       <c r="V13" s="2"/>
       <c r="Y13" s="2"/>
@@ -1007,9 +1027,9 @@
       <c r="Q14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="R14" s="4" t="e">
+      <c r="R14" s="4">
         <f>AVERAGE(R4:R13)</f>
-        <v>#DIV/0!</v>
+        <v>740248.7</v>
       </c>
       <c r="S14" s="4"/>
       <c r="T14" s="11"/>

</xml_diff>

<commit_message>
Updated comparison file to use release values from home, still need to run sequentials in release x64 at uni but I'll worry about that later, won't take long. Trying to get OpenCL working, but I've no got a fucking scooby :smile: :smile: :smile:
</commit_message>
<xml_diff>
--- a/CW2/#Results/#Comparison.xlsx
+++ b/CW2/#Results/#Comparison.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Uni\Year-4\ConcurrentAndParallelSystems\ConcurrentAndParallelSystems\CW2\#Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40168766\Documents\GitHub\ConcurrentAndParallelSystems\CW2\#Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -492,11 +492,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BG31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4:R13"/>
+      <selection activeCell="B4" sqref="B4:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,13 +668,13 @@
     </row>
     <row r="4" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
-        <v>728495</v>
+        <v>355156</v>
       </c>
       <c r="E4" s="2">
-        <v>683505</v>
-      </c>
-      <c r="H4" s="2">
-        <v>683951</v>
+        <v>332321</v>
+      </c>
+      <c r="H4">
+        <v>363086</v>
       </c>
       <c r="L4" s="2"/>
       <c r="O4" s="2"/>
@@ -700,13 +700,13 @@
     </row>
     <row r="5" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
-        <v>740652</v>
+        <v>358755</v>
       </c>
       <c r="E5" s="2">
-        <v>697532</v>
-      </c>
-      <c r="H5" s="2">
-        <v>699999</v>
+        <v>333326</v>
+      </c>
+      <c r="H5">
+        <v>375921</v>
       </c>
       <c r="L5" s="2"/>
       <c r="O5" s="2"/>
@@ -732,13 +732,13 @@
     </row>
     <row r="6" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
-        <v>735935</v>
+        <v>355651</v>
       </c>
       <c r="E6" s="2">
-        <v>688184</v>
-      </c>
-      <c r="H6" s="2">
-        <v>700166</v>
+        <v>330839</v>
+      </c>
+      <c r="H6">
+        <v>373563</v>
       </c>
       <c r="L6" s="2"/>
       <c r="O6" s="2"/>
@@ -764,13 +764,13 @@
     </row>
     <row r="7" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
-        <v>740696</v>
+        <v>356771</v>
       </c>
       <c r="E7" s="2">
-        <v>690818</v>
-      </c>
-      <c r="H7" s="2">
-        <v>701902</v>
+        <v>333033</v>
+      </c>
+      <c r="H7">
+        <v>384730</v>
       </c>
       <c r="L7" s="2"/>
       <c r="O7" s="2"/>
@@ -796,13 +796,13 @@
     </row>
     <row r="8" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
-        <v>729638</v>
+        <v>356573</v>
       </c>
       <c r="E8" s="2">
-        <v>695086</v>
-      </c>
-      <c r="H8" s="2">
-        <v>709870</v>
+        <v>334187</v>
+      </c>
+      <c r="H8">
+        <v>382976</v>
       </c>
       <c r="L8" s="2"/>
       <c r="O8" s="2"/>
@@ -828,13 +828,13 @@
     </row>
     <row r="9" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
-        <v>734381</v>
+        <v>356471</v>
       </c>
       <c r="E9" s="2">
-        <v>689518</v>
-      </c>
-      <c r="H9" s="2">
-        <v>705464</v>
+        <v>331746</v>
+      </c>
+      <c r="H9">
+        <v>379426</v>
       </c>
       <c r="L9" s="2"/>
       <c r="O9" s="2"/>
@@ -860,13 +860,13 @@
     </row>
     <row r="10" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
-        <v>732962</v>
+        <v>357041</v>
       </c>
       <c r="E10" s="2">
-        <v>689554</v>
-      </c>
-      <c r="H10" s="2">
-        <v>711699</v>
+        <v>331386</v>
+      </c>
+      <c r="H10">
+        <v>399030</v>
       </c>
       <c r="L10" s="2"/>
       <c r="O10" s="2"/>
@@ -892,13 +892,13 @@
     </row>
     <row r="11" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
-        <v>734020</v>
+        <v>356491</v>
       </c>
       <c r="E11" s="2">
-        <v>695947</v>
-      </c>
-      <c r="H11" s="2">
-        <v>701693</v>
+        <v>331100</v>
+      </c>
+      <c r="H11">
+        <v>353635</v>
       </c>
       <c r="L11" s="2"/>
       <c r="O11" s="2"/>
@@ -924,13 +924,13 @@
     </row>
     <row r="12" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
-        <v>730931</v>
+        <v>356949</v>
       </c>
       <c r="E12" s="2">
-        <v>690823</v>
-      </c>
-      <c r="H12" s="2">
-        <v>714953</v>
+        <v>332007</v>
+      </c>
+      <c r="H12">
+        <v>361482</v>
       </c>
       <c r="L12" s="2"/>
       <c r="O12" s="2"/>
@@ -956,13 +956,13 @@
     </row>
     <row r="13" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
-        <v>740778</v>
+        <v>359119</v>
       </c>
       <c r="E13" s="2">
-        <v>692842</v>
-      </c>
-      <c r="H13" s="2">
-        <v>706804</v>
+        <v>329878</v>
+      </c>
+      <c r="H13">
+        <v>380121</v>
       </c>
       <c r="L13" s="2"/>
       <c r="O13" s="2"/>
@@ -992,21 +992,21 @@
       </c>
       <c r="B14" s="4">
         <f>AVERAGE(B4:B13)</f>
-        <v>734848.8</v>
+        <v>356897.7</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E14" s="4">
         <f>AVERAGE(E4:E13)</f>
-        <v>691380.9</v>
+        <v>331982.3</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>5</v>
       </c>
       <c r="H14" s="4">
         <f>AVERAGE(H4:H13)</f>
-        <v>703650.1</v>
+        <v>375397</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="11"/>

</xml_diff>

<commit_message>
fixing the fuckup with the comparison file
</commit_message>
<xml_diff>
--- a/CW2/#Results/#Comparison.xlsx
+++ b/CW2/#Results/#Comparison.xlsx
@@ -506,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BG31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L35" sqref="L35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,9 +678,6 @@
       <c r="BG3" s="10"/>
     </row>
     <row r="4" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
-        <v>356763</v>
-      </c>
       <c r="E4" s="2">
         <v>332321</v>
       </c>
@@ -707,9 +704,6 @@
       <c r="BF4" s="2"/>
     </row>
     <row r="5" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="B5" s="2">
-        <v>354597</v>
-      </c>
       <c r="E5" s="2">
         <v>333326</v>
       </c>
@@ -736,9 +730,6 @@
       <c r="BF5" s="2"/>
     </row>
     <row r="6" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="B6" s="2">
-        <v>352081</v>
-      </c>
       <c r="E6" s="2">
         <v>330839</v>
       </c>
@@ -765,9 +756,6 @@
       <c r="BF6" s="2"/>
     </row>
     <row r="7" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="B7" s="2">
-        <v>351276</v>
-      </c>
       <c r="E7" s="2">
         <v>333033</v>
       </c>
@@ -794,9 +782,6 @@
       <c r="BF7" s="2"/>
     </row>
     <row r="8" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="B8" s="2">
-        <v>350255</v>
-      </c>
       <c r="E8" s="2">
         <v>334187</v>
       </c>
@@ -823,9 +808,6 @@
       <c r="BF8" s="2"/>
     </row>
     <row r="9" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="B9" s="2">
-        <v>351346</v>
-      </c>
       <c r="E9" s="2">
         <v>331746</v>
       </c>
@@ -852,9 +834,6 @@
       <c r="BF9" s="2"/>
     </row>
     <row r="10" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="B10" s="2">
-        <v>349813</v>
-      </c>
       <c r="E10" s="2">
         <v>331386</v>
       </c>
@@ -881,9 +860,6 @@
       <c r="BF10" s="2"/>
     </row>
     <row r="11" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="B11" s="2">
-        <v>352911</v>
-      </c>
       <c r="E11" s="2">
         <v>331100</v>
       </c>
@@ -910,9 +886,6 @@
       <c r="BF11" s="2"/>
     </row>
     <row r="12" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="B12" s="2">
-        <v>350557</v>
-      </c>
       <c r="E12" s="2">
         <v>332007</v>
       </c>
@@ -939,9 +912,6 @@
       <c r="BF12" s="2"/>
     </row>
     <row r="13" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="B13" s="2">
-        <v>349949</v>
-      </c>
       <c r="E13" s="2">
         <v>329878</v>
       </c>
@@ -971,9 +941,9 @@
       <c r="A14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="4" t="e">
         <f>AVERAGE(B4:B13)</f>
-        <v>351954.8</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Right comparison file sequentials done both home and away, gg no re
</commit_message>
<xml_diff>
--- a/CW2/#Results/#Comparison.xlsx
+++ b/CW2/#Results/#Comparison.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40168766\Documents\GitHub\ConcurrentAndParallelSystems\CW2\#Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Uni\Year-4\ConcurrentAndParallelSystems\ConcurrentAndParallelSystems\CW2\#Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -503,11 +503,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B13"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,6 +678,9 @@
       <c r="BG3" s="10"/>
     </row>
     <row r="4" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>353650</v>
+      </c>
       <c r="E4" s="2">
         <v>332321</v>
       </c>
@@ -704,6 +707,9 @@
       <c r="BF4" s="2"/>
     </row>
     <row r="5" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>351144</v>
+      </c>
       <c r="E5" s="2">
         <v>333326</v>
       </c>
@@ -730,6 +736,9 @@
       <c r="BF5" s="2"/>
     </row>
     <row r="6" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>351354</v>
+      </c>
       <c r="E6" s="2">
         <v>330839</v>
       </c>
@@ -756,6 +765,9 @@
       <c r="BF6" s="2"/>
     </row>
     <row r="7" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>352388</v>
+      </c>
       <c r="E7" s="2">
         <v>333033</v>
       </c>
@@ -782,6 +794,9 @@
       <c r="BF7" s="2"/>
     </row>
     <row r="8" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>355917</v>
+      </c>
       <c r="E8" s="2">
         <v>334187</v>
       </c>
@@ -808,6 +823,9 @@
       <c r="BF8" s="2"/>
     </row>
     <row r="9" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>353320</v>
+      </c>
       <c r="E9" s="2">
         <v>331746</v>
       </c>
@@ -834,6 +852,9 @@
       <c r="BF9" s="2"/>
     </row>
     <row r="10" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>352149</v>
+      </c>
       <c r="E10" s="2">
         <v>331386</v>
       </c>
@@ -860,6 +881,9 @@
       <c r="BF10" s="2"/>
     </row>
     <row r="11" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>351175</v>
+      </c>
       <c r="E11" s="2">
         <v>331100</v>
       </c>
@@ -886,6 +910,9 @@
       <c r="BF11" s="2"/>
     </row>
     <row r="12" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>350882</v>
+      </c>
       <c r="E12" s="2">
         <v>332007</v>
       </c>
@@ -912,6 +939,9 @@
       <c r="BF12" s="2"/>
     </row>
     <row r="13" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>353572</v>
+      </c>
       <c r="E13" s="2">
         <v>329878</v>
       </c>
@@ -941,9 +971,9 @@
       <c r="A14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="4" t="e">
+      <c r="B14" s="4">
         <f>AVERAGE(B4:B13)</f>
-        <v>#DIV/0!</v>
+        <v>352555.1</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
In the words of Taylor Momsen...
You make me wanna die
</commit_message>
<xml_diff>
--- a/CW2/#Results/#Comparison.xlsx
+++ b/CW2/#Results/#Comparison.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Uni\Year-4\ConcurrentAndParallelSystems\ConcurrentAndParallelSystems\CW2\#Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40168766\Documents\GitHub\ConcurrentAndParallelSystems\CW2\#Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -71,19 +71,19 @@
     <t>CUDA</t>
   </si>
   <si>
-    <t>Parallel for actually marginally slowed down the</t>
+    <t>Parallel for slowed down the Atkin and Sundaram</t>
   </si>
   <si>
-    <t xml:space="preserve"> Sundaram code. I couldn't get it working for Atkin</t>
+    <t>code in the lab, but it did manage to speed up</t>
   </si>
   <si>
-    <t xml:space="preserve"> or Eratosthenes</t>
+    <t>Eratosthenes.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -503,11 +503,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BG31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Adding initial omp results from home
</commit_message>
<xml_diff>
--- a/CW2/#Results/#Comparison.xlsx
+++ b/CW2/#Results/#Comparison.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40168766\Documents\GitHub\ConcurrentAndParallelSystems\CW2\#Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Uni\Year-4\ConcurrentAndParallelSystems\ConcurrentAndParallelSystems\CW2\#Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="19">
   <si>
     <t>Atkin</t>
   </si>
@@ -79,11 +79,14 @@
   <si>
     <t>Eratosthenes.</t>
   </si>
+  <si>
+    <t>Only Sundaram was sped up at home.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -503,11 +506,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BG31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BG36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+      <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,8 +690,15 @@
       <c r="H4">
         <v>363086</v>
       </c>
-      <c r="L4" s="2"/>
-      <c r="O4" s="2"/>
+      <c r="L4">
+        <v>367572</v>
+      </c>
+      <c r="O4" s="2">
+        <v>354232</v>
+      </c>
+      <c r="R4">
+        <v>364832</v>
+      </c>
       <c r="S4" s="2"/>
       <c r="V4" s="2"/>
       <c r="Y4" s="2"/>
@@ -716,8 +726,15 @@
       <c r="H5">
         <v>375921</v>
       </c>
-      <c r="L5" s="2"/>
-      <c r="O5" s="2"/>
+      <c r="L5">
+        <v>367813</v>
+      </c>
+      <c r="O5" s="2">
+        <v>353750</v>
+      </c>
+      <c r="R5">
+        <v>362110</v>
+      </c>
       <c r="S5" s="2"/>
       <c r="V5" s="2"/>
       <c r="Y5" s="2"/>
@@ -745,8 +762,15 @@
       <c r="H6">
         <v>373563</v>
       </c>
-      <c r="L6" s="2"/>
-      <c r="O6" s="2"/>
+      <c r="L6">
+        <v>366714</v>
+      </c>
+      <c r="O6" s="2">
+        <v>354444</v>
+      </c>
+      <c r="R6">
+        <v>363578</v>
+      </c>
       <c r="S6" s="2"/>
       <c r="V6" s="2"/>
       <c r="Y6" s="2"/>
@@ -774,8 +798,15 @@
       <c r="H7">
         <v>384730</v>
       </c>
-      <c r="L7" s="2"/>
-      <c r="O7" s="2"/>
+      <c r="L7">
+        <v>367798</v>
+      </c>
+      <c r="O7" s="2">
+        <v>354779</v>
+      </c>
+      <c r="R7">
+        <v>362158</v>
+      </c>
       <c r="S7" s="2"/>
       <c r="V7" s="2"/>
       <c r="Y7" s="2"/>
@@ -803,8 +834,15 @@
       <c r="H8">
         <v>382976</v>
       </c>
-      <c r="L8" s="2"/>
-      <c r="O8" s="2"/>
+      <c r="L8">
+        <v>365973</v>
+      </c>
+      <c r="O8" s="2">
+        <v>353633</v>
+      </c>
+      <c r="R8">
+        <v>364705</v>
+      </c>
       <c r="S8" s="2"/>
       <c r="V8" s="2"/>
       <c r="Y8" s="2"/>
@@ -832,8 +870,15 @@
       <c r="H9">
         <v>379426</v>
       </c>
-      <c r="L9" s="2"/>
-      <c r="O9" s="2"/>
+      <c r="L9">
+        <v>366098</v>
+      </c>
+      <c r="O9" s="2">
+        <v>353975</v>
+      </c>
+      <c r="R9">
+        <v>365631</v>
+      </c>
       <c r="S9" s="2"/>
       <c r="V9" s="2"/>
       <c r="Y9" s="2"/>
@@ -861,8 +906,15 @@
       <c r="H10">
         <v>399030</v>
       </c>
-      <c r="L10" s="2"/>
-      <c r="O10" s="2"/>
+      <c r="L10">
+        <v>364059</v>
+      </c>
+      <c r="O10" s="2">
+        <v>354619</v>
+      </c>
+      <c r="R10">
+        <v>366666</v>
+      </c>
       <c r="S10" s="2"/>
       <c r="V10" s="2"/>
       <c r="Y10" s="2"/>
@@ -890,8 +942,15 @@
       <c r="H11">
         <v>353635</v>
       </c>
-      <c r="L11" s="2"/>
-      <c r="O11" s="2"/>
+      <c r="L11">
+        <v>366264</v>
+      </c>
+      <c r="O11" s="2">
+        <v>354400</v>
+      </c>
+      <c r="R11">
+        <v>364989</v>
+      </c>
       <c r="S11" s="2"/>
       <c r="V11" s="2"/>
       <c r="Y11" s="2"/>
@@ -919,8 +978,15 @@
       <c r="H12">
         <v>361482</v>
       </c>
-      <c r="L12" s="2"/>
-      <c r="O12" s="2"/>
+      <c r="L12">
+        <v>366725</v>
+      </c>
+      <c r="O12" s="2">
+        <v>354844</v>
+      </c>
+      <c r="R12">
+        <v>364916</v>
+      </c>
       <c r="S12" s="2"/>
       <c r="V12" s="2"/>
       <c r="Y12" s="2"/>
@@ -948,8 +1014,15 @@
       <c r="H13">
         <v>380121</v>
       </c>
-      <c r="L13" s="2"/>
-      <c r="O13" s="2"/>
+      <c r="L13">
+        <v>363865</v>
+      </c>
+      <c r="O13" s="2">
+        <v>353943</v>
+      </c>
+      <c r="R13">
+        <v>366954</v>
+      </c>
       <c r="S13" s="2"/>
       <c r="V13" s="2"/>
       <c r="Y13" s="2"/>
@@ -994,23 +1067,23 @@
       <c r="K14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="L14" s="4" t="e">
+      <c r="L14" s="4">
         <f>AVERAGE(L4:L13)</f>
-        <v>#DIV/0!</v>
+        <v>366288.1</v>
       </c>
       <c r="N14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="O14" s="4" t="e">
+      <c r="O14" s="4">
         <f>AVERAGE(O4:O13)</f>
-        <v>#DIV/0!</v>
+        <v>354261.9</v>
       </c>
       <c r="Q14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="R14" s="4" t="e">
+      <c r="R14" s="4">
         <f>AVERAGE(R4:R13)</f>
-        <v>#DIV/0!</v>
+        <v>364653.9</v>
       </c>
       <c r="S14" s="4"/>
       <c r="T14" s="11"/>
@@ -1727,7 +1800,7 @@
       <c r="E29" s="9"/>
       <c r="H29" s="9"/>
       <c r="I29" s="9"/>
-      <c r="J29" s="11"/>
+      <c r="J29" s="14"/>
       <c r="K29" s="7" t="s">
         <v>15</v>
       </c>
@@ -1735,7 +1808,7 @@
       <c r="O29" s="9"/>
       <c r="R29" s="9"/>
       <c r="S29" s="9"/>
-      <c r="T29" s="11"/>
+      <c r="T29" s="14"/>
       <c r="U29" s="7" t="s">
         <v>9</v>
       </c>
@@ -1743,7 +1816,7 @@
       <c r="Y29" s="9"/>
       <c r="AB29" s="9"/>
       <c r="AC29" s="9"/>
-      <c r="AD29" s="11"/>
+      <c r="AD29" s="14"/>
       <c r="AE29" s="7" t="s">
         <v>9</v>
       </c>
@@ -1751,7 +1824,7 @@
       <c r="AI29" s="9"/>
       <c r="AL29" s="9"/>
       <c r="AM29" s="9"/>
-      <c r="AN29" s="11"/>
+      <c r="AN29" s="14"/>
       <c r="AO29" s="7" t="s">
         <v>9</v>
       </c>
@@ -1759,14 +1832,14 @@
       <c r="AS29" s="9"/>
       <c r="AV29" s="9"/>
       <c r="AW29" s="9"/>
-      <c r="AX29" s="11"/>
+      <c r="AX29" s="14"/>
       <c r="AY29" s="7" t="s">
         <v>9</v>
       </c>
       <c r="AZ29" s="9"/>
       <c r="BC29" s="9"/>
       <c r="BF29" s="9"/>
-      <c r="BG29" s="11"/>
+      <c r="BG29" s="14"/>
     </row>
     <row r="30" spans="1:59" s="7" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
@@ -1776,7 +1849,7 @@
       <c r="E30" s="9"/>
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
-      <c r="J30" s="11"/>
+      <c r="J30" s="14"/>
       <c r="K30" s="7" t="s">
         <v>16</v>
       </c>
@@ -1784,11 +1857,11 @@
       <c r="O30" s="9"/>
       <c r="R30" s="9"/>
       <c r="S30" s="9"/>
-      <c r="T30" s="11"/>
-      <c r="AD30" s="11"/>
-      <c r="AN30" s="11"/>
-      <c r="AX30" s="11"/>
-      <c r="BG30" s="11"/>
+      <c r="T30" s="14"/>
+      <c r="AD30" s="14"/>
+      <c r="AN30" s="14"/>
+      <c r="AX30" s="14"/>
+      <c r="BG30" s="14"/>
     </row>
     <row r="31" spans="1:59" s="7" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B31" s="9"/>
@@ -1805,6 +1878,69 @@
       <c r="AX31" s="14"/>
       <c r="BG31" s="14"/>
     </row>
+    <row r="32" spans="1:59" s="7" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="14"/>
+      <c r="T32" s="14"/>
+      <c r="AD32" s="14"/>
+      <c r="AN32" s="14"/>
+      <c r="AX32" s="14"/>
+      <c r="BG32" s="14"/>
+    </row>
+    <row r="33" spans="2:59" s="7" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="T33" s="14"/>
+      <c r="AD33" s="14"/>
+      <c r="AN33" s="14"/>
+      <c r="AX33" s="14"/>
+      <c r="BG33" s="14"/>
+    </row>
+    <row r="34" spans="2:59" s="7" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="14"/>
+      <c r="T34" s="14"/>
+      <c r="AD34" s="14"/>
+      <c r="AN34" s="14"/>
+      <c r="AX34" s="14"/>
+      <c r="BG34" s="14"/>
+    </row>
+    <row r="35" spans="2:59" s="7" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="14"/>
+      <c r="T35" s="14"/>
+      <c r="AD35" s="14"/>
+      <c r="AN35" s="14"/>
+      <c r="AX35" s="14"/>
+      <c r="BG35" s="14"/>
+    </row>
+    <row r="36" spans="2:59" s="7" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="14"/>
+      <c r="T36" s="14"/>
+      <c r="AD36" s="14"/>
+      <c r="AN36" s="14"/>
+      <c r="AX36" s="14"/>
+      <c r="BG36" s="14"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>